<commit_message>
Adding 5 more gain-only trials
Adding 5 more gain-only trials at the edges (1 very likely to reject, two *must* reject, and two very likely to accept).
</commit_message>
<xml_diff>
--- a/choice_set/novel_choiceset_creation/initialchoiceset.xlsx
+++ b/choice_set/novel_choiceset_creation/initialchoiceset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sokolhessner/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sokolhessner/Documents/gitrepos/clasedecisiontask/choice_set/novel_choiceset_creation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C95B274-BC37-E84D-B66D-A01950A8DE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D72EE-9FE7-B54C-8536-9CF17C1B764A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{39B1200C-5069-4046-B8A1-7519D24964A0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37020" windowHeight="25720" activeTab="4" xr2:uid="{39B1200C-5069-4046-B8A1-7519D24964A0}"/>
   </bookViews>
   <sheets>
     <sheet name="GainLossGeneration" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Choiceset" sheetId="6" r:id="rId5"/>
     <sheet name="Unused - Brainstorming" sheetId="1" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5096,10 +5096,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>GainOnlyGeneration!$P$2:$P$31</c:f>
+              <c:f>GainOnlyGeneration!$P$2:$P$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -5189,16 +5189,31 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1.5730829761119478</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>GainOnlyGeneration!$Q$2:$Q$31</c:f>
+              <c:f>GainOnlyGeneration!$Q$2:$Q$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0.42862199142653634</c:v>
                 </c:pt>
@@ -5287,6 +5302,21 @@
                   <c:v>9.9525657215325225</c:v>
                 </c:pt>
                 <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -5574,10 +5604,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>GainOnlyGeneration!$P$2:$P$31</c:f>
+              <c:f>GainOnlyGeneration!$P$2:$P$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -5667,16 +5697,31 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>1.5730829761119478</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>GainOnlyGeneration!$R$2:$R$31</c:f>
+              <c:f>GainOnlyGeneration!$R$2:$R$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="35"/>
                 <c:pt idx="0">
                   <c:v>0.21431099571326817</c:v>
                 </c:pt>
@@ -5766,6 +5811,21 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.6356943754306037</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15142,7 +15202,7 @@
         <v>-1.1111111111111112</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N31" si="2">H4</f>
+        <f t="shared" ref="N4" si="2">H4</f>
         <v>-1.1111111111111112</v>
       </c>
       <c r="P4">
@@ -15185,7 +15245,7 @@
         <v>-1</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O31" si="4">H5</f>
+        <f t="shared" ref="O5" si="4">H5</f>
         <v>-1</v>
       </c>
       <c r="P5">
@@ -15221,7 +15281,7 @@
         <v>-0.90909090909090917</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N31" si="5">H6</f>
+        <f t="shared" ref="N6" si="5">H6</f>
         <v>-0.90909090909090917</v>
       </c>
       <c r="P6">
@@ -15251,7 +15311,7 @@
         <v>-0.83333333333333337</v>
       </c>
       <c r="O7">
-        <f t="shared" ref="O7:O31" si="6">H7</f>
+        <f t="shared" ref="O7" si="6">H7</f>
         <v>-0.83333333333333337</v>
       </c>
       <c r="P7">
@@ -15288,7 +15348,7 @@
         <v>-0.76923076923076916</v>
       </c>
       <c r="N8">
-        <f t="shared" ref="N8:N31" si="7">H8</f>
+        <f t="shared" ref="N8" si="7">H8</f>
         <v>-0.76923076923076916</v>
       </c>
       <c r="R8">
@@ -15315,7 +15375,7 @@
         <v>-0.71428571428571419</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O31" si="8">H9</f>
+        <f t="shared" ref="O9" si="8">H9</f>
         <v>-0.71428571428571419</v>
       </c>
       <c r="R9">
@@ -15342,7 +15402,7 @@
         <v>-0.66666666666666652</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:N31" si="9">H10</f>
+        <f t="shared" ref="N10" si="9">H10</f>
         <v>-0.66666666666666652</v>
       </c>
       <c r="P10" t="s">
@@ -15372,7 +15432,7 @@
         <v>-0.62499999999999989</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O31" si="10">H11</f>
+        <f t="shared" ref="O11" si="10">H11</f>
         <v>-0.62499999999999989</v>
       </c>
       <c r="R11">
@@ -15399,7 +15459,7 @@
         <v>-0.58823529411764697</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N31" si="11">H12</f>
+        <f t="shared" ref="N12" si="11">H12</f>
         <v>-0.58823529411764697</v>
       </c>
       <c r="R12">
@@ -15426,7 +15486,7 @@
         <v>-0.55555555555555536</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O31" si="12">H13</f>
+        <f t="shared" ref="O13" si="12">H13</f>
         <v>-0.55555555555555536</v>
       </c>
       <c r="R13">
@@ -15453,7 +15513,7 @@
         <v>-0.52631578947368407</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N31" si="13">H14</f>
+        <f t="shared" ref="N14" si="13">H14</f>
         <v>-0.52631578947368407</v>
       </c>
       <c r="R14">
@@ -15480,7 +15540,7 @@
         <v>-0.49999999999999989</v>
       </c>
       <c r="O15">
-        <f t="shared" ref="O15:O31" si="14">H15</f>
+        <f t="shared" ref="O15" si="14">H15</f>
         <v>-0.49999999999999989</v>
       </c>
       <c r="R15">
@@ -15507,7 +15567,7 @@
         <v>-0.47619047619047605</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16:N31" si="16">H16</f>
+        <f t="shared" ref="N16" si="16">H16</f>
         <v>-0.47619047619047605</v>
       </c>
       <c r="R16">
@@ -15534,7 +15594,7 @@
         <v>-0.45454545454545442</v>
       </c>
       <c r="O17">
-        <f t="shared" ref="O17:O31" si="17">H17</f>
+        <f t="shared" ref="O17" si="17">H17</f>
         <v>-0.45454545454545442</v>
       </c>
       <c r="R17">
@@ -15561,7 +15621,7 @@
         <v>-0.43478260869565205</v>
       </c>
       <c r="N18">
-        <f t="shared" ref="N18:N31" si="18">H18</f>
+        <f t="shared" ref="N18" si="18">H18</f>
         <v>-0.43478260869565205</v>
       </c>
       <c r="R18">
@@ -15588,7 +15648,7 @@
         <v>-0.41666666666666652</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O31" si="19">H19</f>
+        <f t="shared" ref="O19" si="19">H19</f>
         <v>-0.41666666666666652</v>
       </c>
       <c r="R19">
@@ -15615,7 +15675,7 @@
         <v>-0.39999999999999986</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20:N31" si="20">H20</f>
+        <f t="shared" ref="N20" si="20">H20</f>
         <v>-0.39999999999999986</v>
       </c>
       <c r="R20">
@@ -15642,7 +15702,7 @@
         <v>-0.35714285714285704</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:O31" si="22">H21</f>
+        <f t="shared" ref="O21" si="22">H21</f>
         <v>-0.35714285714285704</v>
       </c>
       <c r="R21">
@@ -15669,7 +15729,7 @@
         <v>-0.32258064516129026</v>
       </c>
       <c r="N22">
-        <f t="shared" ref="N22:N31" si="23">H22</f>
+        <f t="shared" ref="N22" si="23">H22</f>
         <v>-0.32258064516129026</v>
       </c>
       <c r="R22">
@@ -15696,7 +15756,7 @@
         <v>-0.29411764705882348</v>
       </c>
       <c r="O23">
-        <f t="shared" ref="O23:O31" si="24">H23</f>
+        <f t="shared" ref="O23" si="24">H23</f>
         <v>-0.29411764705882348</v>
       </c>
       <c r="R23">
@@ -15723,7 +15783,7 @@
         <v>-0.27027027027027023</v>
       </c>
       <c r="N24">
-        <f t="shared" ref="N24:N31" si="25">H24</f>
+        <f t="shared" ref="N24" si="25">H24</f>
         <v>-0.27027027027027023</v>
       </c>
       <c r="R24">
@@ -15750,7 +15810,7 @@
         <v>-0.25</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O31" si="26">H25</f>
+        <f t="shared" ref="O25" si="26">H25</f>
         <v>-0.25</v>
       </c>
       <c r="R25">
@@ -15777,7 +15837,7 @@
         <v>-0.21739130434782611</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:N31" si="28">H26</f>
+        <f t="shared" ref="N26" si="28">H26</f>
         <v>-0.21739130434782611</v>
       </c>
       <c r="R26">
@@ -15804,7 +15864,7 @@
         <v>-0.19230769230769235</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:O31" si="29">H27</f>
+        <f t="shared" ref="O27" si="29">H27</f>
         <v>-0.19230769230769235</v>
       </c>
       <c r="R27">
@@ -15831,7 +15891,7 @@
         <v>-0.17241379310344832</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28:N31" si="30">H28</f>
+        <f t="shared" ref="N28" si="30">H28</f>
         <v>-0.17241379310344832</v>
       </c>
       <c r="R28">
@@ -15858,7 +15918,7 @@
         <v>-0.15625000000000003</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:O31" si="31">H29</f>
+        <f t="shared" ref="O29" si="31">H29</f>
         <v>-0.15625000000000003</v>
       </c>
       <c r="R29">
@@ -15885,7 +15945,7 @@
         <v>-0.1428571428571429</v>
       </c>
       <c r="N30">
-        <f t="shared" ref="N30:N31" si="33">H30</f>
+        <f t="shared" ref="N30" si="33">H30</f>
         <v>-0.1428571428571429</v>
       </c>
       <c r="R30">
@@ -17762,10 +17822,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7129CBED-75FE-FE4F-BC90-69ECA6D16CC4}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q31"/>
+      <selection activeCell="P32" sqref="P32:Q36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17865,7 +17925,7 @@
         <v>7</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R31" si="3">Q3/P3</f>
+        <f t="shared" ref="R3:R36" si="3">Q3/P3</f>
         <v>0.26369151912041178</v>
       </c>
     </row>
@@ -17964,7 +18024,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f>E6+B$3</f>
+        <f t="shared" ref="E7:E25" si="5">E6+B$3</f>
         <v>0.75000000000000022</v>
       </c>
       <c r="M7">
@@ -17992,7 +18052,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f>E7+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.77000000000000024</v>
       </c>
       <c r="J8">
@@ -18020,7 +18080,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <f>E8+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.79000000000000026</v>
       </c>
       <c r="M9">
@@ -18048,7 +18108,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f>E9+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.81000000000000028</v>
       </c>
       <c r="J10">
@@ -18076,7 +18136,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <f>E10+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.83000000000000029</v>
       </c>
       <c r="M11">
@@ -18104,7 +18164,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <f>E11+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.85000000000000031</v>
       </c>
       <c r="J12">
@@ -18132,7 +18192,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f>E12+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.87000000000000033</v>
       </c>
       <c r="M13">
@@ -18160,7 +18220,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f>E13+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.89000000000000035</v>
       </c>
       <c r="J14">
@@ -18188,7 +18248,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <f>E14+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.91000000000000036</v>
       </c>
       <c r="M15">
@@ -18216,7 +18276,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f>E15+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.93000000000000038</v>
       </c>
       <c r="J16">
@@ -18244,7 +18304,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f>E16+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.9500000000000004</v>
       </c>
       <c r="M17">
@@ -18272,7 +18332,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <f>E17+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.97000000000000042</v>
       </c>
       <c r="J18">
@@ -18300,7 +18360,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <f>E18+B$3</f>
+        <f t="shared" si="5"/>
         <v>0.99000000000000044</v>
       </c>
       <c r="M19">
@@ -18328,7 +18388,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <f>E19+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.0100000000000005</v>
       </c>
       <c r="J20">
@@ -18356,7 +18416,7 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <f>E20+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.0300000000000005</v>
       </c>
       <c r="M21">
@@ -18384,7 +18444,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f>E21+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.0500000000000005</v>
       </c>
       <c r="J22">
@@ -18412,7 +18472,7 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <f>E22+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.0700000000000005</v>
       </c>
       <c r="M23">
@@ -18440,7 +18500,7 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <f>E23+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.0900000000000005</v>
       </c>
       <c r="J24">
@@ -18468,7 +18528,7 @@
         <v>1</v>
       </c>
       <c r="E25">
-        <f>E24+B$3</f>
+        <f t="shared" si="5"/>
         <v>1.1100000000000005</v>
       </c>
       <c r="M25">
@@ -18496,7 +18556,7 @@
         <v>1</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E26:E27" si="5">E25+B$4</f>
+        <f t="shared" ref="E26:E27" si="6">E25+B$4</f>
         <v>1.1800000000000006</v>
       </c>
       <c r="J26">
@@ -18524,7 +18584,7 @@
         <v>1</v>
       </c>
       <c r="E27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2500000000000007</v>
       </c>
       <c r="M27">
@@ -18657,6 +18717,66 @@
       <c r="R31">
         <f t="shared" si="3"/>
         <v>0.6356943754306037</v>
+      </c>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="P32">
+        <v>7.5</v>
+      </c>
+      <c r="Q32">
+        <v>6</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="16:18" x14ac:dyDescent="0.2">
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="16:18" x14ac:dyDescent="0.2">
+      <c r="P34">
+        <v>9</v>
+      </c>
+      <c r="Q34">
+        <v>9</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="16:18" x14ac:dyDescent="0.2">
+      <c r="P35">
+        <v>15</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="3"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="16:18" x14ac:dyDescent="0.2">
+      <c r="P36">
+        <v>9</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>0.1111111111111111</v>
       </c>
     </row>
   </sheetData>
@@ -18667,10 +18787,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B677BD20-64D3-A347-977A-A26CAB2BEE10}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C31"/>
+      <selection activeCell="A32" sqref="A32:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19013,6 +19133,61 @@
         <v>0</v>
       </c>
       <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>7.5</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
         <v>1</v>
       </c>
     </row>
@@ -19023,10 +19198,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A29162D-6491-3040-93F5-58F97AAC1E5D}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:C121"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="I128" sqref="I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20359,6 +20534,61 @@
         <v>0</v>
       </c>
       <c r="C121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>7.5</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+      <c r="C122">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>5</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+      <c r="C123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>9</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+      <c r="C124">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>15</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>9</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+      <c r="C126">
         <v>1</v>
       </c>
     </row>
@@ -20449,14 +20679,14 @@
         <v>1</v>
       </c>
       <c r="M2" s="1">
-        <f>L2/R$2</f>
+        <f t="shared" ref="M2:M10" si="0">L2/R$2</f>
         <v>0.02</v>
       </c>
       <c r="N2">
         <v>2</v>
       </c>
       <c r="O2">
-        <f>N2/R$2</f>
+        <f t="shared" ref="O2:O10" si="1">N2/R$2</f>
         <v>0.04</v>
       </c>
       <c r="P2">
@@ -20473,7 +20703,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <f>H2</f>
+        <f t="shared" ref="T2:T10" si="2">H2</f>
         <v>-0.02</v>
       </c>
       <c r="U2">
@@ -20493,14 +20723,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="0">A3*H3</f>
+        <f t="shared" ref="B3:B10" si="3">A3*H3</f>
         <v>-0.2</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D64" si="1">B3/A3</f>
+        <f t="shared" ref="D3:D64" si="4">B3/A3</f>
         <v>-0.1</v>
       </c>
       <c r="F3">
@@ -20523,7 +20753,7 @@
         <v>4</v>
       </c>
       <c r="M3" s="1">
-        <f>L3/R$2</f>
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
       <c r="N3">
@@ -20531,7 +20761,7 @@
         <v>5</v>
       </c>
       <c r="O3">
-        <f>N3/R$2</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="P3">
@@ -20539,18 +20769,18 @@
         <v>6</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q10" si="2">P3/R$2</f>
+        <f t="shared" ref="Q3:Q10" si="5">P3/R$2</f>
         <v>0.12</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <f>H3</f>
+        <f t="shared" si="2"/>
         <v>-0.1</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U28" si="3">-1/T3</f>
+        <f t="shared" ref="U3:U28" si="6">-1/T3</f>
         <v>10</v>
       </c>
       <c r="AC3" t="s">
@@ -20564,7 +20794,7 @@
         <v>0.65</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AF28" si="4">-1/AE3</f>
+        <f t="shared" ref="AF3:AF28" si="7">-1/AE3</f>
         <v>-1.5384615384615383</v>
       </c>
     </row>
@@ -20573,64 +20803,64 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.48000000000000004</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.24000000000000002</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H10" si="5">H3-$M4</f>
+        <f t="shared" ref="H4:H10" si="8">H3-$M4</f>
         <v>-0.24000000000000002</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I10" si="6">I3-$O4</f>
+        <f t="shared" ref="I4:I10" si="9">I3-$O4</f>
         <v>-0.30000000000000004</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J10" si="7">J3-$Q4</f>
+        <f t="shared" ref="J4:J10" si="10">J3-$Q4</f>
         <v>-0.36</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L10" si="8">L3+3</f>
+        <f t="shared" ref="L4:L10" si="11">L3+3</f>
         <v>7</v>
       </c>
       <c r="M4" s="1">
-        <f>L4/R$2</f>
+        <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N10" si="9">N3+3</f>
+        <f t="shared" ref="N4:N10" si="12">N3+3</f>
         <v>8</v>
       </c>
       <c r="O4">
-        <f>N4/R$2</f>
+        <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P10" si="10">P3+3</f>
+        <f t="shared" ref="P4:P10" si="13">P3+3</f>
         <v>9</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.18</v>
       </c>
       <c r="S4">
         <v>1</v>
       </c>
       <c r="T4">
-        <f>H4</f>
+        <f t="shared" si="2"/>
         <v>-0.24000000000000002</v>
       </c>
       <c r="U4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.1666666666666661</v>
       </c>
       <c r="AC4" t="s">
@@ -20640,11 +20870,11 @@
         <v>0.1</v>
       </c>
       <c r="AE4">
-        <f t="shared" ref="AE4:AE28" si="11">AE3+AD$3</f>
+        <f t="shared" ref="AE4:AE7" si="14">AE3+AD$3</f>
         <v>0.8</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.25</v>
       </c>
     </row>
@@ -20653,64 +20883,64 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.88000000000000012</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.44000000000000006</v>
       </c>
       <c r="F5">
         <v>7</v>
       </c>
       <c r="H5">
+        <f t="shared" si="8"/>
+        <v>-0.44000000000000006</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="9"/>
+        <v>-0.52</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="10"/>
+        <v>-0.6</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="13"/>
+        <v>12</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="5"/>
-        <v>-0.44000000000000006</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="6"/>
-        <v>-0.52</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="7"/>
-        <v>-0.6</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="M5" s="1">
-        <f>L5/R$2</f>
-        <v>0.2</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="O5">
-        <f>N5/R$2</f>
-        <v>0.22</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="2"/>
         <v>0.24</v>
       </c>
       <c r="S5">
         <v>1</v>
       </c>
       <c r="T5">
-        <f>H5</f>
+        <f t="shared" si="2"/>
         <v>-0.44000000000000006</v>
       </c>
       <c r="U5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.2727272727272725</v>
       </c>
       <c r="AC5" t="s">
@@ -20720,11 +20950,11 @@
         <v>0.25</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.95000000000000007</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.0526315789473684</v>
       </c>
     </row>
@@ -20733,64 +20963,64 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.4000000000000001</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.70000000000000007</v>
       </c>
       <c r="F6">
         <v>8</v>
       </c>
       <c r="H6">
+        <f t="shared" si="8"/>
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="9"/>
+        <v>-0.8</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="10"/>
+        <v>-0.89999999999999991</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="5"/>
-        <v>-0.70000000000000007</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="6"/>
-        <v>-0.8</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="7"/>
-        <v>-0.89999999999999991</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="M6" s="1">
-        <f>L6/R$2</f>
-        <v>0.26</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="9"/>
-        <v>14</v>
-      </c>
-      <c r="O6">
-        <f>N6/R$2</f>
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="S6">
         <v>1</v>
       </c>
       <c r="T6">
-        <f>H6</f>
+        <f t="shared" si="2"/>
         <v>-0.70000000000000007</v>
       </c>
       <c r="U6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.4285714285714284</v>
       </c>
       <c r="AC6" t="s">
@@ -20800,11 +21030,11 @@
         <v>0.4</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.90909090909090906</v>
       </c>
     </row>
@@ -20813,72 +21043,72 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.04</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.02</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
       <c r="H7">
+        <f t="shared" si="8"/>
+        <v>-1.02</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="9"/>
+        <v>-1.1400000000000001</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="10"/>
+        <v>-1.2599999999999998</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="12"/>
+        <v>17</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>0.34</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="13"/>
+        <v>18</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="5"/>
-        <v>-1.02</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="6"/>
-        <v>-1.1400000000000001</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="7"/>
-        <v>-1.2599999999999998</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="M7" s="1">
-        <f>L7/R$2</f>
-        <v>0.32</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="9"/>
-        <v>17</v>
-      </c>
-      <c r="O7">
-        <f>N7/R$2</f>
-        <v>0.34</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
       <c r="S7">
         <v>1</v>
       </c>
       <c r="T7">
-        <f>H7</f>
+        <f t="shared" si="2"/>
         <v>-1.02</v>
       </c>
       <c r="U7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.98039215686274506</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1.25</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.8</v>
       </c>
     </row>
@@ -20887,64 +21117,64 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.8</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.4</v>
       </c>
       <c r="F8">
         <v>12</v>
       </c>
       <c r="H8">
+        <f t="shared" si="8"/>
+        <v>-1.4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="9"/>
+        <v>-1.54</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="10"/>
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="11"/>
+        <v>19</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="13"/>
+        <v>21</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="5"/>
-        <v>-1.4</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="6"/>
-        <v>-1.54</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="7"/>
-        <v>-1.6799999999999997</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="8"/>
-        <v>19</v>
-      </c>
-      <c r="M8" s="1">
-        <f>L8/R$2</f>
-        <v>0.38</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="9"/>
-        <v>20</v>
-      </c>
-      <c r="O8">
-        <f>N8/R$2</f>
-        <v>0.4</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="10"/>
-        <v>21</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="2"/>
         <v>0.42</v>
       </c>
       <c r="S8">
         <v>1</v>
       </c>
       <c r="T8">
-        <f>H8</f>
+        <f t="shared" si="2"/>
         <v>-1.4</v>
       </c>
       <c r="U8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="AE8">
@@ -20952,7 +21182,7 @@
         <v>1.35</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.7407407407407407</v>
       </c>
     </row>
@@ -20961,69 +21191,69 @@
         <v>2</v>
       </c>
       <c r="B9">
+        <f t="shared" si="3"/>
+        <v>-3.6799999999999997</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="4"/>
+        <v>-1.8399999999999999</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="8"/>
+        <v>-1.8399999999999999</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="10"/>
+        <v>-2.1599999999999997</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="11"/>
+        <v>22</v>
+      </c>
+      <c r="M9" s="1">
         <f t="shared" si="0"/>
-        <v>-3.6799999999999997</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+        <v>0.44</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="12"/>
+        <v>23</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="1"/>
-        <v>-1.8399999999999999</v>
-      </c>
-      <c r="H9">
+        <v>0.46</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="5"/>
-        <v>-1.8399999999999999</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="6"/>
-        <v>-2</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="7"/>
-        <v>-2.1599999999999997</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="8"/>
-        <v>22</v>
-      </c>
-      <c r="M9" s="1">
-        <f>L9/R$2</f>
-        <v>0.44</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="9"/>
-        <v>23</v>
-      </c>
-      <c r="O9">
-        <f>N9/R$2</f>
-        <v>0.46</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="10"/>
-        <v>24</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
         <v>0.48</v>
       </c>
       <c r="S9">
         <v>1</v>
       </c>
       <c r="T9">
-        <f>H9</f>
+        <f t="shared" si="2"/>
         <v>-1.8399999999999999</v>
       </c>
       <c r="U9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.5434782608695653</v>
       </c>
       <c r="AE9">
-        <f t="shared" ref="AE9:AE15" si="12">AE8+AD$4</f>
+        <f t="shared" ref="AE9:AE15" si="15">AE8+AD$4</f>
         <v>1.4500000000000002</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.68965517241379304</v>
       </c>
     </row>
@@ -21032,69 +21262,69 @@
         <v>2</v>
       </c>
       <c r="B10">
+        <f t="shared" si="3"/>
+        <v>-4.68</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="4"/>
+        <v>-2.34</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="8"/>
+        <v>-2.34</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="9"/>
+        <v>-2.52</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="10"/>
+        <v>-2.6999999999999997</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="11"/>
+        <v>25</v>
+      </c>
+      <c r="M10" s="1">
         <f t="shared" si="0"/>
-        <v>-4.68</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="O10">
         <f t="shared" si="1"/>
-        <v>-2.34</v>
-      </c>
-      <c r="H10">
+        <v>0.52</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="13"/>
+        <v>27</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="5"/>
-        <v>-2.34</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="6"/>
-        <v>-2.52</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="7"/>
-        <v>-2.6999999999999997</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="8"/>
-        <v>25</v>
-      </c>
-      <c r="M10" s="1">
-        <f>L10/R$2</f>
-        <v>0.5</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="9"/>
-        <v>26</v>
-      </c>
-      <c r="O10">
-        <f>N10/R$2</f>
-        <v>0.52</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="10"/>
-        <v>27</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="2"/>
         <v>0.54</v>
       </c>
       <c r="S10">
         <v>1</v>
       </c>
       <c r="T10">
-        <f>H10</f>
+        <f t="shared" si="2"/>
         <v>-2.34</v>
       </c>
       <c r="U10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.42735042735042739</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.5500000000000003</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.64516129032258052</v>
       </c>
     </row>
@@ -21103,33 +21333,33 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <f>A11*I2</f>
+        <f t="shared" ref="B11:B19" si="16">A11*I2</f>
         <v>-0.16</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.04</v>
       </c>
       <c r="S11">
         <v>1</v>
       </c>
       <c r="T11">
-        <f>I2</f>
+        <f t="shared" ref="T11:T19" si="17">I2</f>
         <v>-0.04</v>
       </c>
       <c r="U11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.6500000000000004</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.60606060606060597</v>
       </c>
     </row>
@@ -21138,33 +21368,33 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <f>A12*I3</f>
+        <f t="shared" si="16"/>
         <v>-0.56000000000000005</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.14000000000000001</v>
       </c>
       <c r="S12">
         <v>1</v>
       </c>
       <c r="T12">
-        <f>I3</f>
+        <f t="shared" si="17"/>
         <v>-0.14000000000000001</v>
       </c>
       <c r="U12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.1428571428571423</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.7500000000000004</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.57142857142857129</v>
       </c>
     </row>
@@ -21173,33 +21403,33 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <f>A13*I4</f>
+        <f t="shared" si="16"/>
         <v>-1.2000000000000002</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="S13">
         <v>1</v>
       </c>
       <c r="T13">
-        <f>I4</f>
+        <f t="shared" si="17"/>
         <v>-0.30000000000000004</v>
       </c>
       <c r="U13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.333333333333333</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.8500000000000005</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.54054054054054035</v>
       </c>
     </row>
@@ -21208,33 +21438,33 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <f>A14*I5</f>
+        <f t="shared" si="16"/>
         <v>-2.08</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.52</v>
       </c>
       <c r="S14">
         <v>1</v>
       </c>
       <c r="T14">
-        <f>I5</f>
+        <f t="shared" si="17"/>
         <v>-0.52</v>
       </c>
       <c r="U14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.9230769230769229</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.9500000000000006</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.51282051282051266</v>
       </c>
     </row>
@@ -21243,33 +21473,33 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <f>A15*I6</f>
+        <f t="shared" si="16"/>
         <v>-3.2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.8</v>
       </c>
       <c r="S15">
         <v>1</v>
       </c>
       <c r="T15">
-        <f>I6</f>
+        <f t="shared" si="17"/>
         <v>-0.8</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.25</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.0500000000000007</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.48780487804878031</v>
       </c>
     </row>
@@ -21278,33 +21508,33 @@
         <v>4</v>
       </c>
       <c r="B16">
-        <f>A16*I7</f>
+        <f t="shared" si="16"/>
         <v>-4.5600000000000005</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.1400000000000001</v>
       </c>
       <c r="S16">
         <v>1</v>
       </c>
       <c r="T16">
-        <f>I7</f>
+        <f t="shared" si="17"/>
         <v>-1.1400000000000001</v>
       </c>
       <c r="U16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.8771929824561403</v>
       </c>
       <c r="AE16">
-        <f t="shared" ref="AE11:AE20" si="13">AE15+AD$4</f>
+        <f t="shared" ref="AE16:AE18" si="18">AE15+AD$4</f>
         <v>2.1500000000000008</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.46511627906976727</v>
       </c>
     </row>
@@ -21313,33 +21543,33 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <f>A17*I8</f>
+        <f t="shared" si="16"/>
         <v>-6.16</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.54</v>
       </c>
       <c r="S17">
         <v>1</v>
       </c>
       <c r="T17">
-        <f>I8</f>
+        <f t="shared" si="17"/>
         <v>-1.54</v>
       </c>
       <c r="U17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.64935064935064934</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2.2500000000000009</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.44444444444444425</v>
       </c>
     </row>
@@ -21348,33 +21578,33 @@
         <v>4</v>
       </c>
       <c r="B18">
-        <f>A18*I9</f>
+        <f t="shared" si="16"/>
         <v>-8</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="S18">
         <v>1</v>
       </c>
       <c r="T18">
-        <f>I9</f>
+        <f t="shared" si="17"/>
         <v>-2</v>
       </c>
       <c r="U18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.5</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>2.350000000000001</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.42553191489361686</v>
       </c>
     </row>
@@ -21383,25 +21613,25 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <f>A19*I10</f>
+        <f t="shared" si="16"/>
         <v>-10.08</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.52</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19">
-        <f>I10</f>
+        <f t="shared" si="17"/>
         <v>-2.52</v>
       </c>
       <c r="U19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.3968253968253968</v>
       </c>
       <c r="AE19">
@@ -21409,7 +21639,7 @@
         <v>2.4500000000000011</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.40816326530612229</v>
       </c>
     </row>
@@ -21418,33 +21648,33 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <f>A20*J2</f>
+        <f t="shared" ref="B20:B28" si="19">A20*J2</f>
         <v>-0.3</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.06</v>
       </c>
       <c r="S20">
         <v>1</v>
       </c>
       <c r="T20">
-        <f>J2</f>
+        <f t="shared" ref="T20:T28" si="20">J2</f>
         <v>-0.06</v>
       </c>
       <c r="U20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16.666666666666668</v>
       </c>
       <c r="AE20">
-        <f t="shared" ref="AE20:AE21" si="14">AE19+AD$5</f>
+        <f t="shared" ref="AE20:AE21" si="21">AE19+AD$5</f>
         <v>2.7000000000000011</v>
       </c>
       <c r="AF20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.37037037037037024</v>
       </c>
     </row>
@@ -21453,33 +21683,33 @@
         <v>5</v>
       </c>
       <c r="B21">
-        <f>A21*J3</f>
+        <f t="shared" si="19"/>
         <v>-0.89999999999999991</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
       <c r="S21">
         <v>1</v>
       </c>
       <c r="T21">
-        <f>J3</f>
+        <f t="shared" si="20"/>
         <v>-0.18</v>
       </c>
       <c r="U21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.5555555555555554</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>2.9500000000000011</v>
       </c>
       <c r="AF21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.3389830508474575</v>
       </c>
     </row>
@@ -21488,25 +21718,25 @@
         <v>5</v>
       </c>
       <c r="B22">
-        <f>A22*J4</f>
+        <f t="shared" si="19"/>
         <v>-1.7999999999999998</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.36</v>
       </c>
       <c r="S22">
         <v>1</v>
       </c>
       <c r="T22">
-        <f>J4</f>
+        <f t="shared" si="20"/>
         <v>-0.36</v>
       </c>
       <c r="U22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.7777777777777777</v>
       </c>
       <c r="AE22">
@@ -21514,7 +21744,7 @@
         <v>3.2000000000000011</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.31249999999999989</v>
       </c>
     </row>
@@ -21523,33 +21753,33 @@
         <v>5</v>
       </c>
       <c r="B23">
-        <f>A23*J5</f>
+        <f t="shared" si="19"/>
         <v>-3</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.6</v>
       </c>
       <c r="S23">
         <v>1</v>
       </c>
       <c r="T23">
-        <f>J5</f>
+        <f t="shared" si="20"/>
         <v>-0.6</v>
       </c>
       <c r="U23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="AE23">
-        <f t="shared" ref="AE23:AE28" si="15">AE22+AD$5</f>
+        <f t="shared" ref="AE23:AE24" si="22">AE22+AD$5</f>
         <v>3.4500000000000011</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.28985507246376802</v>
       </c>
     </row>
@@ -21558,33 +21788,33 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <f>A24*J6</f>
+        <f t="shared" si="19"/>
         <v>-4.5</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.9</v>
       </c>
       <c r="S24">
         <v>1</v>
       </c>
       <c r="T24">
-        <f>J6</f>
+        <f t="shared" si="20"/>
         <v>-0.89999999999999991</v>
       </c>
       <c r="U24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.1111111111111112</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="22"/>
         <v>3.7000000000000011</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.27027027027027017</v>
       </c>
     </row>
@@ -21593,25 +21823,25 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <f>A25*J7</f>
+        <f t="shared" si="19"/>
         <v>-6.2999999999999989</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.2599999999999998</v>
       </c>
       <c r="S25">
         <v>1</v>
       </c>
       <c r="T25">
-        <f>J7</f>
+        <f t="shared" si="20"/>
         <v>-1.2599999999999998</v>
       </c>
       <c r="U25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.79365079365079383</v>
       </c>
       <c r="AE25">
@@ -21619,7 +21849,7 @@
         <v>4.1000000000000014</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.24390243902439016</v>
       </c>
     </row>
@@ -21628,33 +21858,33 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <f>A26*J8</f>
+        <f t="shared" si="19"/>
         <v>-8.3999999999999986</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.6799999999999997</v>
       </c>
       <c r="S26">
         <v>1</v>
       </c>
       <c r="T26">
-        <f>J8</f>
+        <f t="shared" si="20"/>
         <v>-1.6799999999999997</v>
       </c>
       <c r="U26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.59523809523809534</v>
       </c>
       <c r="AE26">
-        <f t="shared" ref="AE26:AE28" si="16">AE25+AD$6</f>
+        <f t="shared" ref="AE26:AE28" si="23">AE25+AD$6</f>
         <v>4.5000000000000018</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.22222222222222213</v>
       </c>
     </row>
@@ -21663,33 +21893,33 @@
         <v>5</v>
       </c>
       <c r="B27">
-        <f>A27*J9</f>
+        <f t="shared" si="19"/>
         <v>-10.799999999999999</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.1599999999999997</v>
       </c>
       <c r="S27">
         <v>1</v>
       </c>
       <c r="T27">
-        <f>J9</f>
+        <f t="shared" si="20"/>
         <v>-2.1599999999999997</v>
       </c>
       <c r="U27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.46296296296296302</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>4.9000000000000021</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.20408163265306115</v>
       </c>
     </row>
@@ -21698,33 +21928,33 @@
         <v>5</v>
       </c>
       <c r="B28">
-        <f>A28*J10</f>
+        <f t="shared" si="19"/>
         <v>-13.499999999999998</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.6999999999999997</v>
       </c>
       <c r="S28">
         <v>1</v>
       </c>
       <c r="T28">
-        <f>J10</f>
+        <f t="shared" si="20"/>
         <v>-2.6999999999999997</v>
       </c>
       <c r="U28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.37037037037037041</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="23"/>
         <v>5.3000000000000025</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.18867924528301877</v>
       </c>
     </row>
@@ -21740,7 +21970,7 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.02</v>
       </c>
     </row>
@@ -21749,14 +21979,14 @@
         <v>7</v>
       </c>
       <c r="B30">
-        <f t="shared" ref="B30:B37" si="17">A30*H3</f>
+        <f t="shared" ref="B30:B37" si="24">A30*H3</f>
         <v>-0.70000000000000007</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.1</v>
       </c>
       <c r="U30">
@@ -21769,14 +21999,14 @@
         <v>7</v>
       </c>
       <c r="B31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-1.6800000000000002</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.24000000000000002</v>
       </c>
       <c r="U31">
@@ -21789,14 +22019,14 @@
         <v>7</v>
       </c>
       <c r="B32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-3.0800000000000005</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.44000000000000006</v>
       </c>
     </row>
@@ -21805,14 +22035,14 @@
         <v>7</v>
       </c>
       <c r="B33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-4.9000000000000004</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.70000000000000007</v>
       </c>
     </row>
@@ -21821,14 +22051,14 @@
         <v>7</v>
       </c>
       <c r="B34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-7.1400000000000006</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.02</v>
       </c>
     </row>
@@ -21837,14 +22067,14 @@
         <v>7</v>
       </c>
       <c r="B35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-9.7999999999999989</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.4</v>
       </c>
     </row>
@@ -21853,14 +22083,14 @@
         <v>7</v>
       </c>
       <c r="B36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-12.879999999999999</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.8399999999999999</v>
       </c>
     </row>
@@ -21869,14 +22099,14 @@
         <v>7</v>
       </c>
       <c r="B37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="24"/>
         <v>-16.38</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.34</v>
       </c>
     </row>
@@ -21892,7 +22122,7 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.04</v>
       </c>
     </row>
@@ -21901,14 +22131,14 @@
         <v>8</v>
       </c>
       <c r="B39">
-        <f t="shared" ref="B39:B46" si="18">A39*I3</f>
+        <f t="shared" ref="B39:B46" si="25">A39*I3</f>
         <v>-1.1200000000000001</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.14000000000000001</v>
       </c>
     </row>
@@ -21917,14 +22147,14 @@
         <v>8</v>
       </c>
       <c r="B40">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-2.4000000000000004</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.30000000000000004</v>
       </c>
     </row>
@@ -21933,14 +22163,14 @@
         <v>8</v>
       </c>
       <c r="B41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-4.16</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.52</v>
       </c>
     </row>
@@ -21949,14 +22179,14 @@
         <v>8</v>
       </c>
       <c r="B42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-6.4</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.8</v>
       </c>
     </row>
@@ -21965,14 +22195,14 @@
         <v>8</v>
       </c>
       <c r="B43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-9.120000000000001</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.1400000000000001</v>
       </c>
     </row>
@@ -21981,14 +22211,14 @@
         <v>8</v>
       </c>
       <c r="B44">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-12.32</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.54</v>
       </c>
     </row>
@@ -21997,14 +22227,14 @@
         <v>8</v>
       </c>
       <c r="B45">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-16</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
     </row>
@@ -22013,14 +22243,14 @@
         <v>8</v>
       </c>
       <c r="B46">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>-20.16</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.52</v>
       </c>
     </row>
@@ -22036,7 +22266,7 @@
         <v>0</v>
       </c>
       <c r="D47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.06</v>
       </c>
     </row>
@@ -22045,14 +22275,14 @@
         <v>10</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:B55" si="19">A48*J3</f>
+        <f t="shared" ref="B48:B55" si="26">A48*J3</f>
         <v>-1.7999999999999998</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.18</v>
       </c>
     </row>
@@ -22061,14 +22291,14 @@
         <v>10</v>
       </c>
       <c r="B49">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-3.5999999999999996</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.36</v>
       </c>
     </row>
@@ -22077,14 +22307,14 @@
         <v>10</v>
       </c>
       <c r="B50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-6</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.6</v>
       </c>
     </row>
@@ -22093,14 +22323,14 @@
         <v>10</v>
       </c>
       <c r="B51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-9</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.9</v>
       </c>
     </row>
@@ -22109,14 +22339,14 @@
         <v>10</v>
       </c>
       <c r="B52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-12.599999999999998</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.2599999999999998</v>
       </c>
     </row>
@@ -22125,14 +22355,14 @@
         <v>10</v>
       </c>
       <c r="B53">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-16.799999999999997</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.6799999999999997</v>
       </c>
     </row>
@@ -22141,14 +22371,14 @@
         <v>10</v>
       </c>
       <c r="B54">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-21.599999999999998</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.1599999999999997</v>
       </c>
     </row>
@@ -22157,14 +22387,14 @@
         <v>10</v>
       </c>
       <c r="B55">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>-26.999999999999996</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.6999999999999997</v>
       </c>
     </row>
@@ -22180,7 +22410,7 @@
         <v>0</v>
       </c>
       <c r="D56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.02</v>
       </c>
     </row>
@@ -22189,14 +22419,14 @@
         <v>12</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B64" si="20">A57*H3</f>
+        <f t="shared" ref="B57:B64" si="27">A57*H3</f>
         <v>-1.2000000000000002</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.10000000000000002</v>
       </c>
     </row>
@@ -22205,14 +22435,14 @@
         <v>12</v>
       </c>
       <c r="B58">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-2.8800000000000003</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.24000000000000002</v>
       </c>
     </row>
@@ -22221,14 +22451,14 @@
         <v>12</v>
       </c>
       <c r="B59">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-5.2800000000000011</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.44000000000000011</v>
       </c>
     </row>
@@ -22237,14 +22467,14 @@
         <v>12</v>
       </c>
       <c r="B60">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-8.4</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.70000000000000007</v>
       </c>
     </row>
@@ -22253,14 +22483,14 @@
         <v>12</v>
       </c>
       <c r="B61">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-12.24</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.02</v>
       </c>
     </row>
@@ -22269,14 +22499,14 @@
         <v>12</v>
       </c>
       <c r="B62">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-16.799999999999997</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.3999999999999997</v>
       </c>
     </row>
@@ -22285,14 +22515,14 @@
         <v>12</v>
       </c>
       <c r="B63">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-22.08</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-1.8399999999999999</v>
       </c>
     </row>
@@ -22301,14 +22531,14 @@
         <v>12</v>
       </c>
       <c r="B64">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>-28.08</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.34</v>
       </c>
     </row>

</xml_diff>